<commit_message>
completed nested loop example
</commit_message>
<xml_diff>
--- a/Students/Chris/Chris_class_schedule.xlsx
+++ b/Students/Chris/Chris_class_schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepo\balee323\TeachingCode\Chris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepo\balee323\TeachingCode\Students\Chris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EF4974-3592-420A-B054-B86000EFB3AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F9C88F-4ABE-4314-B18E-C7A128498905}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA54AE47-6627-40DE-9821-82EC4BBC49CD}"/>
   </bookViews>
@@ -116,9 +116,6 @@
     <t>Fri 15May20</t>
   </si>
   <si>
-    <t>Learning Arrays!  |  Arrays Part1 HW  | Go over HW4</t>
-  </si>
-  <si>
     <t>Sun 17May20</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Review Pass by value and Pass by reference  &amp; Net reading assignment (read handouts -&gt; Programming Lecture 1.docx). | Assignments: HW4 (using functions that pass by value vs Reference) </t>
+  </si>
+  <si>
+    <t>Learning Arrays!  |  Arrays Part1 HW  | Go over HW3</t>
   </si>
 </sst>
 </file>
@@ -396,28 +396,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6017DF5C-742D-463B-B71C-3447463530F2}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:B30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +748,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -764,7 +764,7 @@
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -772,37 +772,37 @@
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="12"/>
     </row>
     <row r="6" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="13"/>
     </row>
     <row r="7" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:2" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -810,13 +810,13 @@
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="19"/>
     </row>
     <row r="11" spans="1:2" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>11</v>
       </c>
     </row>
@@ -824,13 +824,13 @@
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="17"/>
     </row>
     <row r="13" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="18" t="s">
         <v>13</v>
       </c>
     </row>
@@ -838,13 +838,13 @@
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="13"/>
+      <c r="B14" s="19"/>
     </row>
     <row r="15" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -852,13 +852,13 @@
       <c r="A16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="17"/>
     </row>
     <row r="17" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="18" t="s">
         <v>17</v>
       </c>
     </row>
@@ -866,13 +866,13 @@
       <c r="A18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="13"/>
+      <c r="B18" s="19"/>
     </row>
     <row r="19" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -880,13 +880,13 @@
       <c r="A20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="18" t="s">
         <v>21</v>
       </c>
     </row>
@@ -894,81 +894,81 @@
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="13"/>
+      <c r="B22" s="19"/>
     </row>
     <row r="23" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>51</v>
+      <c r="B23" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="15"/>
+      <c r="B24" s="17"/>
     </row>
     <row r="25" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>52</v>
+      <c r="B25" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="19"/>
     </row>
     <row r="27" spans="1:2" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>53</v>
+      <c r="B27" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="17"/>
     </row>
     <row r="29" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>54</v>
+      <c r="B29" s="18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="17"/>
+      <c r="B30" s="19"/>
     </row>
     <row r="31" spans="1:2" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>27</v>
+      <c r="B31" s="16" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="17"/>
     </row>
     <row r="33" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="8"/>
     </row>
@@ -977,158 +977,158 @@
         <v>3</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="19"/>
+      <c r="B36" s="15"/>
     </row>
     <row r="37" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="17"/>
+      <c r="B38" s="13"/>
     </row>
     <row r="39" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="19"/>
+      <c r="B40" s="15"/>
     </row>
     <row r="41" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="17"/>
+      <c r="B42" s="13"/>
     </row>
     <row r="43" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="19"/>
+      <c r="B44" s="15"/>
     </row>
     <row r="45" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="17"/>
+      <c r="B46" s="13"/>
     </row>
     <row r="47" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="18"/>
+        <v>41</v>
+      </c>
+      <c r="B47" s="14"/>
     </row>
     <row r="48" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="19"/>
+      <c r="B48" s="15"/>
     </row>
     <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="17"/>
+      <c r="B50" s="13"/>
     </row>
     <row r="51" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="18"/>
+        <v>44</v>
+      </c>
+      <c r="B51" s="14"/>
     </row>
     <row r="52" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="19"/>
+      <c r="B52" s="15"/>
     </row>
     <row r="53" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="17"/>
+      <c r="B54" s="13"/>
     </row>
     <row r="55" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="19"/>
+      <c r="B56" s="15"/>
     </row>
     <row r="57" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
@@ -1223,14 +1223,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
@@ -1243,13 +1241,16 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated chris's lecture schedule
</commit_message>
<xml_diff>
--- a/Students/Chris/Chris_class_schedule.xlsx
+++ b/Students/Chris/Chris_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepo\balee323\TeachingCode\Students\Chris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F9C88F-4ABE-4314-B18E-C7A128498905}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FB709C-2802-484F-A794-CFE7B8297CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA54AE47-6627-40DE-9821-82EC4BBC49CD}"/>
   </bookViews>
@@ -119,27 +119,15 @@
     <t>Sun 17May20</t>
   </si>
   <si>
-    <t>Doing stuff with Arrays in a loop | Arrays Part2 HW  | Go over Arrays Part1</t>
-  </si>
-  <si>
     <t>Tue 19May20</t>
   </si>
   <si>
-    <t>Nested Loops!   | Arrays Part3 HW   |  Go over Arrays Part2</t>
-  </si>
-  <si>
     <t>Fri 22May20</t>
   </si>
   <si>
-    <t>Lists!  Life just got easier.  |  Lists HW</t>
-  </si>
-  <si>
     <t>Sun 24May20</t>
   </si>
   <si>
-    <t xml:space="preserve">IO -&gt; let’s mess with some text files!  </t>
-  </si>
-  <si>
     <t>Tue 26May20</t>
   </si>
   <si>
@@ -155,9 +143,6 @@
     <t>Sun 31May20</t>
   </si>
   <si>
-    <t>Stacks and Queues</t>
-  </si>
-  <si>
     <t>Tue 2Jun20</t>
   </si>
   <si>
@@ -177,9 +162,6 @@
   </si>
   <si>
     <t>Fri 12Jun20</t>
-  </si>
-  <si>
-    <t>OOP</t>
   </si>
   <si>
     <r>
@@ -218,6 +200,24 @@
   </si>
   <si>
     <t>Learning Arrays!  |  Arrays Part1 HW  | Go over HW3</t>
+  </si>
+  <si>
+    <t>Doing stuff with Arrays in a loop &amp; Nested Loops!   | Arrays Part2 HW &amp;&amp; Arrays Part3  | Go over Arrays Part1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lists!  Life just got easier.  |  Lists HW |  Go over Arrays Part2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Crash-cource on OOP</t>
+  </si>
+  <si>
+    <t>IO -&gt; let’s mess with some text files!  &amp; Try/catch  (HW -&gt; Load files and print duplicate numbers)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning GUI stuff -&gt; GUI HW </t>
+  </si>
+  <si>
+    <t>Stacks and Queues   -&gt;  HW  -&gt;  create a Queing system  (using a GUI)</t>
   </si>
 </sst>
 </file>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6017DF5C-742D-463B-B71C-3447463530F2}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:B32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +748,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -901,7 +901,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -915,7 +915,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -929,7 +929,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -957,7 +957,7 @@
         <v>26</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -972,20 +972,20 @@
       </c>
       <c r="B33" s="8"/>
     </row>
-    <row r="34" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -996,10 +996,10 @@
     </row>
     <row r="37" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1010,10 +1010,10 @@
     </row>
     <row r="39" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1024,10 +1024,10 @@
     </row>
     <row r="41" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1038,10 +1038,10 @@
     </row>
     <row r="43" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1052,10 +1052,10 @@
     </row>
     <row r="45" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1066,9 +1066,11 @@
     </row>
     <row r="47" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="14"/>
+        <v>36</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="48" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
@@ -1078,10 +1080,10 @@
     </row>
     <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1092,7 +1094,7 @@
     </row>
     <row r="51" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B51" s="14"/>
     </row>
@@ -1104,10 +1106,10 @@
     </row>
     <row r="53" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1118,11 +1120,9 @@
     </row>
     <row r="55" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>48</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B55" s="14"/>
     </row>
     <row r="56" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">

</xml_diff>

<commit_message>
made change to schedule
</commit_message>
<xml_diff>
--- a/Students/Chris/Chris_class_schedule.xlsx
+++ b/Students/Chris/Chris_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepo\balee323\TeachingCode\Students\Chris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FB709C-2802-484F-A794-CFE7B8297CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24C2AFA-B771-44FC-A2BE-58D0CD8756EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA54AE47-6627-40DE-9821-82EC4BBC49CD}"/>
   </bookViews>
@@ -363,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -396,6 +396,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -408,16 +420,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -736,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6017DF5C-742D-463B-B71C-3447463530F2}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:B52"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +767,7 @@
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -772,37 +775,37 @@
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="15"/>
     </row>
     <row r="5" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="18"/>
     </row>
     <row r="8" spans="1:2" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -810,13 +813,13 @@
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="13"/>
     </row>
     <row r="11" spans="1:2" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -824,13 +827,13 @@
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="15"/>
     </row>
     <row r="13" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -838,13 +841,13 @@
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="13"/>
     </row>
     <row r="15" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -852,13 +855,13 @@
       <c r="A16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="15"/>
     </row>
     <row r="17" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -866,13 +869,13 @@
       <c r="A18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="13"/>
     </row>
     <row r="19" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -880,13 +883,13 @@
       <c r="A20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="17"/>
+      <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -894,13 +897,13 @@
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="19"/>
+      <c r="B22" s="13"/>
     </row>
     <row r="23" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -908,13 +911,13 @@
       <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="17"/>
+      <c r="B24" s="15"/>
     </row>
     <row r="25" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="12" t="s">
         <v>45</v>
       </c>
     </row>
@@ -922,13 +925,13 @@
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="13"/>
     </row>
     <row r="27" spans="1:2" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="14" t="s">
         <v>46</v>
       </c>
     </row>
@@ -936,13 +939,13 @@
       <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="15"/>
     </row>
     <row r="29" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -950,13 +953,13 @@
       <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="19"/>
+      <c r="B30" s="13"/>
     </row>
     <row r="31" spans="1:2" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="14" t="s">
         <v>48</v>
       </c>
     </row>
@@ -964,7 +967,7 @@
       <c r="A32" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="17"/>
+      <c r="B32" s="15"/>
     </row>
     <row r="33" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -976,7 +979,7 @@
       <c r="A34" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="20" t="s">
         <v>49</v>
       </c>
     </row>
@@ -984,7 +987,7 @@
       <c r="A35" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -992,13 +995,13 @@
       <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="19"/>
     </row>
     <row r="37" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1006,13 +1009,13 @@
       <c r="A38" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="13"/>
+      <c r="B38" s="17"/>
     </row>
     <row r="39" spans="1:2" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="18" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1020,13 +1023,13 @@
       <c r="A40" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="15"/>
+      <c r="B40" s="19"/>
     </row>
     <row r="41" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="16" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1034,13 +1037,13 @@
       <c r="A42" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="13"/>
+      <c r="B42" s="17"/>
     </row>
     <row r="43" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="18" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1048,13 +1051,13 @@
       <c r="A44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="15"/>
+      <c r="B44" s="19"/>
     </row>
     <row r="45" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="16" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1062,13 +1065,13 @@
       <c r="A46" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="13"/>
+      <c r="B46" s="17"/>
     </row>
     <row r="47" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1076,13 +1079,13 @@
       <c r="A48" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="15"/>
+      <c r="B48" s="19"/>
     </row>
     <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1090,25 +1093,25 @@
       <c r="A50" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="13"/>
+      <c r="B50" s="17"/>
     </row>
     <row r="51" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B51" s="14"/>
+      <c r="B51" s="18"/>
     </row>
     <row r="52" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="15"/>
+      <c r="B52" s="19"/>
     </row>
     <row r="53" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="16" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1116,19 +1119,19 @@
       <c r="A54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="13"/>
+      <c r="B54" s="17"/>
     </row>
     <row r="55" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B55" s="14"/>
+      <c r="B55" s="18"/>
     </row>
     <row r="56" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="15"/>
+      <c r="B56" s="19"/>
     </row>
     <row r="57" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
@@ -1223,12 +1226,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
@@ -1241,14 +1246,12 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added flat-file parser to SimpleFileEditor
</commit_message>
<xml_diff>
--- a/Students/Chris/Chris_class_schedule.xlsx
+++ b/Students/Chris/Chris_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepo\balee323\TeachingCode\Students\Chris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC25B645-F45B-4294-9E8C-6FF25E9253C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB72902-010E-4AAC-88E4-8F2DF28A7FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA54AE47-6627-40DE-9821-82EC4BBC49CD}"/>
   </bookViews>
@@ -196,9 +196,6 @@
     <t>Doing stuff with Arrays in a loop &amp; Nested Loops!   | Arrays Part2 HW &amp;&amp; Arrays Part3  | Go over Arrays Part1</t>
   </si>
   <si>
-    <t>Crash-cource on OOP</t>
-  </si>
-  <si>
     <t xml:space="preserve"> IO -&gt; let’s mess with some text files!  &amp; Try/catch &amp; Lists!  Life just got easier.  |  Lists HW, HW -&gt; Load files and print duplicate numbers |  Go over Arrays Part 1,2 &amp; 3</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>More on String!   Substrings, split methods, contains, IndexOf, ToCharArray, ToLower/ToUpper, Length, Trim, | HW -&gt;  create console text file editor (save&amp;load, file name, date, and content [split method])</t>
+  </si>
+  <si>
+    <t>Crash-course on OOP</t>
   </si>
 </sst>
 </file>
@@ -402,6 +402,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -412,18 +424,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6017DF5C-742D-463B-B71C-3447463530F2}">
   <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B36"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +770,7 @@
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -778,37 +778,37 @@
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="16"/>
     </row>
     <row r="5" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13"/>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
     </row>
     <row r="8" spans="1:2" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="20"/>
     </row>
     <row r="9" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -816,13 +816,13 @@
       <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="20"/>
+      <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:2" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -830,13 +830,13 @@
       <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="16"/>
     </row>
     <row r="13" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -844,13 +844,13 @@
       <c r="A14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="20"/>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -858,13 +858,13 @@
       <c r="A16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="16"/>
     </row>
     <row r="17" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="13" t="s">
         <v>17</v>
       </c>
     </row>
@@ -872,13 +872,13 @@
       <c r="A18" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="20"/>
+      <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -886,13 +886,13 @@
       <c r="A20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="18"/>
+      <c r="B20" s="16"/>
     </row>
     <row r="21" spans="1:2" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -900,13 +900,13 @@
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="20"/>
+      <c r="B22" s="14"/>
     </row>
     <row r="23" spans="1:2" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -914,13 +914,13 @@
       <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="18"/>
+      <c r="B24" s="16"/>
     </row>
     <row r="25" spans="1:2" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -928,13 +928,13 @@
       <c r="A26" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="20"/>
+      <c r="B26" s="14"/>
     </row>
     <row r="27" spans="1:2" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -942,13 +942,13 @@
       <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="18"/>
+      <c r="B28" s="16"/>
     </row>
     <row r="29" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="13" t="s">
         <v>44</v>
       </c>
     </row>
@@ -956,13 +956,13 @@
       <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="20"/>
+      <c r="B30" s="14"/>
     </row>
     <row r="31" spans="1:2" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="15" t="s">
         <v>45</v>
       </c>
     </row>
@@ -970,7 +970,7 @@
       <c r="A32" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="18"/>
+      <c r="B32" s="16"/>
     </row>
     <row r="33" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
@@ -991,7 +991,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1005,7 +1005,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1018,105 +1018,105 @@
       <c r="A39" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>47</v>
+      <c r="B39" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="16"/>
+      <c r="B40" s="20"/>
     </row>
     <row r="41" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="13" t="s">
-        <v>54</v>
+      <c r="B41" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="14"/>
+      <c r="B42" s="18"/>
     </row>
     <row r="43" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="15" t="s">
-        <v>49</v>
+      <c r="B43" s="19" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="16"/>
+      <c r="B44" s="20"/>
     </row>
     <row r="45" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="13" t="s">
-        <v>50</v>
+      <c r="B45" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="14"/>
+      <c r="B46" s="18"/>
     </row>
     <row r="47" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="15" t="s">
-        <v>51</v>
+      <c r="B47" s="19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="16"/>
+      <c r="B48" s="20"/>
     </row>
     <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="13" t="s">
-        <v>52</v>
+      <c r="B49" s="17" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="14"/>
+      <c r="B50" s="18"/>
     </row>
     <row r="51" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="15" t="s">
-        <v>53</v>
+      <c r="B51" s="19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="16"/>
+      <c r="B52" s="20"/>
     </row>
     <row r="53" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1124,19 +1124,19 @@
       <c r="A54" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="14"/>
+      <c r="B54" s="18"/>
     </row>
     <row r="55" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="15"/>
+      <c r="B55" s="19"/>
     </row>
     <row r="56" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="16"/>
+      <c r="B56" s="20"/>
     </row>
     <row r="57" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
@@ -1231,12 +1231,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
@@ -1249,14 +1251,12 @@
     <mergeCell ref="B31:B32"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added comments to OOP lecture code
</commit_message>
<xml_diff>
--- a/Students/Chris/Chris_class_schedule.xlsx
+++ b/Students/Chris/Chris_class_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepo\balee323\TeachingCode\Students\Chris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB72902-010E-4AAC-88E4-8F2DF28A7FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34EF967-97F3-4C7F-899F-B70CEBC204EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA54AE47-6627-40DE-9821-82EC4BBC49CD}"/>
   </bookViews>
@@ -743,7 +743,7 @@
   <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:B42"/>
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>